<commit_message>
added some LLM generated accessibility fixes
</commit_message>
<xml_diff>
--- a/Ryan_Bell_LLM_Sheet.xlsx
+++ b/Ryan_Bell_LLM_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Creation_Sheet" sheetId="1" state="visible" r:id="rId3"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t xml:space="preserve">WAVE errors (https://wave.webaim.org/)</t>
   </si>
@@ -246,10 +246,10 @@
     <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/chatgpt/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Ask Codi</t>
+    <t xml:space="preserve">n/a</t>
   </si>
   <si>
-    <t xml:space="preserve">n/a</t>
+    <t xml:space="preserve">Ask Codi</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/index.html</t>
@@ -261,13 +261,28 @@
     <t xml:space="preserve">You</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.blackbox.ai/share/51850356-5da9-47f3-89bb-cd0163aa6369</t>
+    <t xml:space="preserve">https://you.com/search?q=Please+generate+a+portfolio+website+for+an+entry+level+software+developer+who+is+experienced+in...&amp;cid=c1_60af780d-a3d6-40fc-98af-3041c08fdd82&amp;tbm=youchat</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/you/index.html</t>
   </si>
   <si>
     <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/you/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 X Very low contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4 Distinguishable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrast (Enhanced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAA</t>
   </si>
   <si>
     <t xml:space="preserve">Google Bard (Gemini)</t>
@@ -306,16 +321,13 @@
     <t xml:space="preserve">3.1 Readable</t>
   </si>
   <si>
-    <t xml:space="preserve">WCAG 2.0</t>
+    <t xml:space="preserve">3.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Success Criteria 3.1.1 Language of Page (A)</t>
+    <t xml:space="preserve">Success Criteria 3.1.1 Language of Page</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 X Device dependent event handler</t>
   </si>
   <si>
     <t xml:space="preserve">Microsoft Copilot</t>
@@ -327,7 +339,7 @@
     <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html</t>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot/index.html</t>
   </si>
   <si>
     <t xml:space="preserve">Tabnine</t>
@@ -395,9 +407,6 @@
     <t xml:space="preserve">1 X Linked image missing alternative text</t>
   </si>
   <si>
-    <t xml:space="preserve">1.4 Distinguishable</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.4.4</t>
   </si>
   <si>
@@ -408,6 +417,12 @@
   </si>
   <si>
     <t xml:space="preserve">1 X Very low contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://you.com/search?q=I+ran+the+code+above+through+a+couple+of+online+accessibility+checkers+and+got+the+following+errors%3A...&amp;cid=c1_923b64a7-af9d-4755-82de-033a643fd86e&amp;tbm=youchat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html</t>
   </si>
 </sst>
 </file>
@@ -707,11 +722,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,8 +997,8 @@
   </sheetPr>
   <dimension ref="A1:O906"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1093,7 +1108,9 @@
       <c r="H3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="J3" s="15"/>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
@@ -1158,10 +1175,10 @@
       <c r="C7" s="9"/>
       <c r="D7" s="11"/>
       <c r="E7" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>25</v>
@@ -1169,7 +1186,9 @@
       <c r="H7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -1245,13 +1264,27 @@
       <c r="H11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
+      <c r="I11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
@@ -1310,18 +1343,20 @@
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="20" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
-      <c r="I15" s="15"/>
+      <c r="I15" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
@@ -1386,16 +1421,16 @@
       <c r="C19" s="9"/>
       <c r="D19" s="11"/>
       <c r="E19" s="20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="G19" s="22" t="s">
-        <v>36</v>
+      <c r="G19" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -1462,34 +1497,34 @@
       <c r="C23" s="9"/>
       <c r="D23" s="11"/>
       <c r="E23" s="20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
-      <c r="I23" s="23" t="s">
-        <v>41</v>
+      <c r="I23" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="J23" s="15" t="n">
         <v>1</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
-      <c r="M23" s="23" t="s">
-        <v>44</v>
+      <c r="M23" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O23" s="15" t="n">
         <v>2</v>
@@ -1504,12 +1539,8 @@
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
-      <c r="I24" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="15" t="n">
-        <v>1</v>
-      </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
@@ -1556,24 +1587,34 @@
       <c r="C27" s="9"/>
       <c r="D27" s="11"/>
       <c r="E27" s="20" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
+      <c r="K27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9"/>
@@ -1632,16 +1673,16 @@
       <c r="C31" s="9"/>
       <c r="D31" s="11"/>
       <c r="E31" s="20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -1708,16 +1749,16 @@
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -1784,16 +1825,16 @@
       <c r="C39" s="9"/>
       <c r="D39" s="11"/>
       <c r="E39" s="20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -1860,16 +1901,16 @@
       <c r="C43" s="9"/>
       <c r="D43" s="11"/>
       <c r="E43" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -1936,16 +1977,16 @@
       <c r="C47" s="9"/>
       <c r="D47" s="11"/>
       <c r="E47" s="20" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -3535,7 +3576,7 @@
     <hyperlink ref="G7" r:id="rId6" display="https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/index.html"/>
     <hyperlink ref="H7" r:id="rId7" display="https://raian621.github.io/llm-prompting-assignment/ask-codi/index.html"/>
     <hyperlink ref="E11" r:id="rId8" display="You"/>
-    <hyperlink ref="F11" r:id="rId9" display="https://www.blackbox.ai/share/51850356-5da9-47f3-89bb-cd0163aa6369"/>
+    <hyperlink ref="F11" r:id="rId9" display="https://you.com/search?q=Please+generate+a+portfolio+website+for+an+entry+level+software+developer+who+is+experienced+in...&amp;cid=c1_60af780d-a3d6-40fc-98af-3041c08fdd82&amp;tbm=youchat"/>
     <hyperlink ref="G11" r:id="rId10" display="https://github.com/raian621/llm-prompting-assignment/tree/main/you/index.html"/>
     <hyperlink ref="H11" r:id="rId11" display="https://raian621.github.io/llm-prompting-assignment/you/index.html"/>
     <hyperlink ref="E15" r:id="rId12" display="Google Bard (Gemini)"/>
@@ -3551,7 +3592,7 @@
     <hyperlink ref="E27" r:id="rId22" display="Microsoft Copilot"/>
     <hyperlink ref="F27" r:id="rId23" display="https://copilot.microsoft.com/sl/eGI3mUKzzbM"/>
     <hyperlink ref="G27" r:id="rId24" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
-    <hyperlink ref="H27" r:id="rId25" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
+    <hyperlink ref="H27" r:id="rId25" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot/index.html"/>
     <hyperlink ref="E31" r:id="rId26" display="Tabnine"/>
     <hyperlink ref="G31" r:id="rId27" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
     <hyperlink ref="H31" r:id="rId28" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
@@ -3587,8 +3628,8 @@
   </sheetPr>
   <dimension ref="A1:X895"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3647,7 +3688,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
@@ -3697,18 +3738,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" s="13" t="s">
         <v>21</v>
       </c>
@@ -3716,22 +3759,22 @@
         <v>22</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="J3" s="15" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="2"/>
@@ -3754,7 +3797,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="12"/>
       <c r="I4" s="19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>1</v>
@@ -3832,9 +3875,11 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="12"/>
       <c r="G7" s="21" t="s">
         <v>25</v>
       </c>
@@ -3944,7 +3989,9 @@
       <c r="E11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="G11" s="12" t="s">
         <v>29</v>
       </c>
@@ -4052,14 +4099,16 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="20" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
@@ -4162,14 +4211,16 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="22" t="s">
-        <v>36</v>
+      <c r="F19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -4195,8 +4246,8 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -4221,8 +4272,8 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -4272,14 +4323,16 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="G23" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -4382,14 +4435,14 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="20" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -4492,14 +4545,14 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -4602,14 +4655,14 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -4712,14 +4765,14 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -4822,14 +4875,14 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -4932,14 +4985,14 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="20" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -27070,35 +27123,36 @@
     <hyperlink ref="G7" r:id="rId5" display="https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/index.html"/>
     <hyperlink ref="H7" r:id="rId6" display="https://raian621.github.io/llm-prompting-assignment/ask-codi/index.html"/>
     <hyperlink ref="E11" r:id="rId7" display="You"/>
-    <hyperlink ref="G11" r:id="rId8" display="https://github.com/raian621/llm-prompting-assignment/tree/main/you/index.html"/>
-    <hyperlink ref="H11" r:id="rId9" display="https://raian621.github.io/llm-prompting-assignment/you/index.html"/>
-    <hyperlink ref="E15" r:id="rId10" display="Google Bard (Gemini)"/>
-    <hyperlink ref="G15" r:id="rId11" display="https://github.com/raian621/llm-prompting-assignment/tree/main/gemini/index.html"/>
-    <hyperlink ref="H15" r:id="rId12" display="https://raian621.github.io/llm-prompting-assignment/gemini/index.html"/>
-    <hyperlink ref="E19" r:id="rId13" display="GitHub Copilot"/>
-    <hyperlink ref="G19" r:id="rId14" display="https://github.com/raian621/llm-prompting-assignment/tree/main/github-copilot/index.html"/>
-    <hyperlink ref="H19" r:id="rId15" display="https://raian621.github.io/llm-prompting-assignment/github-copilot/index.html"/>
-    <hyperlink ref="E23" r:id="rId16" display="Amazom Whisperer"/>
-    <hyperlink ref="G23" r:id="rId17" display="https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/index.html"/>
-    <hyperlink ref="H23" r:id="rId18" display="https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/index.html"/>
-    <hyperlink ref="E27" r:id="rId19" display="Microsoft Copilot"/>
-    <hyperlink ref="G27" r:id="rId20" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
-    <hyperlink ref="H27" r:id="rId21" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
-    <hyperlink ref="E31" r:id="rId22" display="Tabnine"/>
-    <hyperlink ref="G31" r:id="rId23" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H31" r:id="rId24" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
-    <hyperlink ref="E35" r:id="rId25" display="Codeium"/>
-    <hyperlink ref="G35" r:id="rId26" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/index.html"/>
-    <hyperlink ref="H35" r:id="rId27" display="https://raian621.github.io/llm-prompting-assignment/codeium/index.html"/>
-    <hyperlink ref="E39" r:id="rId28" display="Phind"/>
-    <hyperlink ref="G39" r:id="rId29" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H39" r:id="rId30" display="https://raian621.github.io/llm-prompting-assignment/phind/index.html"/>
-    <hyperlink ref="E43" r:id="rId31" display="blackbox"/>
-    <hyperlink ref="G43" r:id="rId32" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/index.html"/>
-    <hyperlink ref="H43" r:id="rId33" display="https://raian621.github.io/llm-prompting-assignment/blackbox/index.html"/>
-    <hyperlink ref="E47" r:id="rId34" display="double"/>
-    <hyperlink ref="G47" r:id="rId35" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/index.html"/>
-    <hyperlink ref="H47" r:id="rId36" display="https://raian621.github.io/llm-prompting-assignment/double/index.html"/>
+    <hyperlink ref="F11" r:id="rId8" display="https://you.com/search?q=I+ran+the+code+above+through+a+couple+of+online+accessibility+checkers+and+got+the+following+errors%3A...&amp;cid=c1_923b64a7-af9d-4755-82de-033a643fd86e&amp;tbm=youchat"/>
+    <hyperlink ref="G11" r:id="rId9" display="https://github.com/raian621/llm-prompting-assignment/tree/main/you/index.html"/>
+    <hyperlink ref="H11" r:id="rId10" display="https://raian621.github.io/llm-prompting-assignment/you/index.html"/>
+    <hyperlink ref="E15" r:id="rId11" display="Google Bard (Gemini)"/>
+    <hyperlink ref="G15" r:id="rId12" display="https://github.com/raian621/llm-prompting-assignment/tree/main/gemini/index.html"/>
+    <hyperlink ref="H15" r:id="rId13" display="https://raian621.github.io/llm-prompting-assignment/gemini/index.html"/>
+    <hyperlink ref="E19" r:id="rId14" display="GitHub Copilot"/>
+    <hyperlink ref="G19" r:id="rId15" display="https://github.com/raian621/llm-prompting-assignment/tree/main/github-copilot/index.html"/>
+    <hyperlink ref="H19" r:id="rId16" display="https://raian621.github.io/llm-prompting-assignment/github-copilot/index.html"/>
+    <hyperlink ref="E23" r:id="rId17" display="Amazom Whisperer"/>
+    <hyperlink ref="G23" r:id="rId18" display="https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/index.html"/>
+    <hyperlink ref="H23" r:id="rId19" display="https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/index.html"/>
+    <hyperlink ref="E27" r:id="rId20" display="Microsoft Copilot"/>
+    <hyperlink ref="G27" r:id="rId21" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
+    <hyperlink ref="H27" r:id="rId22" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
+    <hyperlink ref="E31" r:id="rId23" display="Tabnine"/>
+    <hyperlink ref="G31" r:id="rId24" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
+    <hyperlink ref="H31" r:id="rId25" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
+    <hyperlink ref="E35" r:id="rId26" display="Codeium"/>
+    <hyperlink ref="G35" r:id="rId27" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/index.html"/>
+    <hyperlink ref="H35" r:id="rId28" display="https://raian621.github.io/llm-prompting-assignment/codeium/index.html"/>
+    <hyperlink ref="E39" r:id="rId29" display="Phind"/>
+    <hyperlink ref="G39" r:id="rId30" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
+    <hyperlink ref="H39" r:id="rId31" display="https://raian621.github.io/llm-prompting-assignment/phind/index.html"/>
+    <hyperlink ref="E43" r:id="rId32" display="blackbox"/>
+    <hyperlink ref="G43" r:id="rId33" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/index.html"/>
+    <hyperlink ref="H43" r:id="rId34" display="https://raian621.github.io/llm-prompting-assignment/blackbox/index.html"/>
+    <hyperlink ref="E47" r:id="rId35" display="double"/>
+    <hyperlink ref="G47" r:id="rId36" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/index.html"/>
+    <hyperlink ref="H47" r:id="rId37" display="https://raian621.github.io/llm-prompting-assignment/double/index.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -27107,6 +27161,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId37"/>
+  <legacyDrawing r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
got tabnine to work, fixed most of the accessibility issues
</commit_message>
<xml_diff>
--- a/Ryan_Bell_LLM_Sheet.xlsx
+++ b/Ryan_Bell_LLM_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creation_Sheet" sheetId="1" state="visible" r:id="rId3"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
   <si>
     <t xml:space="preserve">WAVE errors (https://wave.webaim.org/)</t>
   </si>
@@ -246,10 +246,13 @@
     <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/chatgpt/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">n/a</t>
+    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">Ask Codi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/index.html</t>
@@ -324,7 +327,7 @@
     <t xml:space="preserve">3.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Success Criteria 3.1.1 Language of Page</t>
+    <t xml:space="preserve">Language of Page</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -422,7 +425,13 @@
     <t xml:space="preserve">https://you.com/search?q=I+ran+the+code+above+through+a+couple+of+online+accessibility+checkers+and+got+the+following+errors%3A...&amp;cid=c1_923b64a7-af9d-4755-82de-033a643fd86e&amp;tbm=youchat</t>
   </si>
   <si>
+    <t xml:space="preserve">https://copilot.microsoft.com/sl/gMszgQ8X9eC</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.blackbox.ai/share/3d6c22e2-66e1-487e-b651-f20b36edee82</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1006,8 @@
   </sheetPr>
   <dimension ref="A1:O906"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,7 +1121,9 @@
         <v>23</v>
       </c>
       <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="K3" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
       <c r="N3" s="15"/>
@@ -1178,19 +1189,21 @@
         <v>24</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -1253,34 +1266,34 @@
       <c r="C11" s="9"/>
       <c r="D11" s="11"/>
       <c r="E11" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J11" s="15" t="n">
         <v>3</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O11" s="15" t="n">
         <v>3</v>
@@ -1343,22 +1356,24 @@
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
+      <c r="K15" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
@@ -1421,24 +1436,36 @@
       <c r="C19" s="9"/>
       <c r="D19" s="11"/>
       <c r="E19" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="23" t="s">
-        <v>41</v>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15" t="s">
+        <v>33</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>42</v>
+      <c r="L19" s="15" t="s">
+        <v>34</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
+      <c r="M19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
@@ -1497,34 +1524,34 @@
       <c r="C23" s="9"/>
       <c r="D23" s="11"/>
       <c r="E23" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J23" s="15" t="n">
         <v>1</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O23" s="15" t="n">
         <v>2</v>
@@ -1587,30 +1614,32 @@
       <c r="C27" s="9"/>
       <c r="D27" s="11"/>
       <c r="E27" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
-      <c r="I27" s="15"/>
+      <c r="I27" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O27" s="15" t="n">
         <v>4</v>
@@ -1673,16 +1702,16 @@
       <c r="C31" s="9"/>
       <c r="D31" s="11"/>
       <c r="E31" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -1749,20 +1778,24 @@
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>60</v>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15" t="s">
+        <v>23</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
@@ -1825,20 +1858,24 @@
       <c r="C39" s="9"/>
       <c r="D39" s="11"/>
       <c r="E39" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
-      <c r="I39" s="15"/>
+      <c r="I39" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
+      <c r="K39" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
@@ -1901,23 +1938,33 @@
       <c r="C43" s="9"/>
       <c r="D43" s="11"/>
       <c r="E43" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
-      <c r="I43" s="15"/>
+      <c r="I43" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
+      <c r="K43" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L43" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M43" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="O43" s="15"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1977,16 +2024,16 @@
       <c r="C47" s="9"/>
       <c r="D47" s="11"/>
       <c r="E47" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -3628,8 +3675,8 @@
   </sheetPr>
   <dimension ref="A1:X895"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3688,7 +3735,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
@@ -3738,19 +3785,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>21</v>
@@ -3759,22 +3806,22 @@
         <v>22</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J3" s="15" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="2"/>
@@ -3797,7 +3844,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="12"/>
       <c r="I4" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>1</v>
@@ -3878,13 +3925,13 @@
         <v>24</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -3987,16 +4034,16 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -4099,16 +4146,16 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
@@ -4211,16 +4258,16 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -4323,16 +4370,16 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -4435,14 +4482,16 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="G27" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -4545,14 +4594,14 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -4655,14 +4704,16 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="F35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="H35" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -4765,14 +4816,16 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
-      <c r="F39" s="12"/>
+      <c r="F39" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G39" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -4875,14 +4928,16 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
-      <c r="F43" s="12"/>
+      <c r="F43" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="G43" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -4985,14 +5040,16 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12" t="s">
         <v>70</v>
       </c>
+      <c r="F47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="H47" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -27136,23 +27193,24 @@
     <hyperlink ref="G23" r:id="rId18" display="https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/index.html"/>
     <hyperlink ref="H23" r:id="rId19" display="https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/index.html"/>
     <hyperlink ref="E27" r:id="rId20" display="Microsoft Copilot"/>
-    <hyperlink ref="G27" r:id="rId21" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
-    <hyperlink ref="H27" r:id="rId22" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
-    <hyperlink ref="E31" r:id="rId23" display="Tabnine"/>
-    <hyperlink ref="G31" r:id="rId24" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H31" r:id="rId25" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
-    <hyperlink ref="E35" r:id="rId26" display="Codeium"/>
-    <hyperlink ref="G35" r:id="rId27" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/index.html"/>
-    <hyperlink ref="H35" r:id="rId28" display="https://raian621.github.io/llm-prompting-assignment/codeium/index.html"/>
-    <hyperlink ref="E39" r:id="rId29" display="Phind"/>
-    <hyperlink ref="G39" r:id="rId30" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H39" r:id="rId31" display="https://raian621.github.io/llm-prompting-assignment/phind/index.html"/>
-    <hyperlink ref="E43" r:id="rId32" display="blackbox"/>
-    <hyperlink ref="G43" r:id="rId33" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/index.html"/>
-    <hyperlink ref="H43" r:id="rId34" display="https://raian621.github.io/llm-prompting-assignment/blackbox/index.html"/>
-    <hyperlink ref="E47" r:id="rId35" display="double"/>
-    <hyperlink ref="G47" r:id="rId36" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/index.html"/>
-    <hyperlink ref="H47" r:id="rId37" display="https://raian621.github.io/llm-prompting-assignment/double/index.html"/>
+    <hyperlink ref="F27" r:id="rId21" display="https://copilot.microsoft.com/sl/gMszgQ8X9eC"/>
+    <hyperlink ref="G27" r:id="rId22" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
+    <hyperlink ref="H27" r:id="rId23" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
+    <hyperlink ref="E31" r:id="rId24" display="Tabnine"/>
+    <hyperlink ref="G31" r:id="rId25" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
+    <hyperlink ref="H31" r:id="rId26" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
+    <hyperlink ref="E35" r:id="rId27" display="Codeium"/>
+    <hyperlink ref="G35" r:id="rId28" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/index.html"/>
+    <hyperlink ref="H35" r:id="rId29" display="https://raian621.github.io/llm-prompting-assignment/codeium/index.html"/>
+    <hyperlink ref="E39" r:id="rId30" display="Phind"/>
+    <hyperlink ref="G39" r:id="rId31" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
+    <hyperlink ref="H39" r:id="rId32" display="https://raian621.github.io/llm-prompting-assignment/phind/index.html"/>
+    <hyperlink ref="E43" r:id="rId33" display="blackbox"/>
+    <hyperlink ref="G43" r:id="rId34" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/index.html"/>
+    <hyperlink ref="H43" r:id="rId35" display="https://raian621.github.io/llm-prompting-assignment/blackbox/index.html"/>
+    <hyperlink ref="E47" r:id="rId36" display="double"/>
+    <hyperlink ref="G47" r:id="rId37" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/index.html"/>
+    <hyperlink ref="H47" r:id="rId38" display="https://raian621.github.io/llm-prompting-assignment/double/index.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -27161,6 +27219,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
got double to work
</commit_message>
<xml_diff>
--- a/Ryan_Bell_LLM_Sheet.xlsx
+++ b/Ryan_Bell_LLM_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Creation_Sheet" sheetId="1" state="visible" r:id="rId3"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="107">
   <si>
     <t xml:space="preserve">WAVE errors (https://wave.webaim.org/)</t>
   </si>
@@ -407,6 +407,12 @@
 Can you please fix the mentioned errors in the above code and provide the corrected source code?</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/chatgpt/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/chatgpt/fixed.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 X Linked image missing alternative text</t>
   </si>
   <si>
@@ -422,16 +428,76 @@
     <t xml:space="preserve">1 X Very low contrast</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/ask-codi/fixed.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://you.com/search?q=I+ran+the+code+above+through+a+couple+of+online+accessibility+checkers+and+got+the+following+errors%3A...&amp;cid=c1_923b64a7-af9d-4755-82de-033a643fd86e&amp;tbm=youchat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/you/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/you/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/gemini/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/gemini/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/github-copilot/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/github-copilot/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/fixed.html</t>
   </si>
   <si>
     <t xml:space="preserve">https://copilot.microsoft.com/sl/gMszgQ8X9eC</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html</t>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/microsoft-copilot/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/tabnine/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/codeium/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/phind/fixed.html</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.blackbox.ai/share/3d6c22e2-66e1-487e-b651-f20b36edee82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/blackbox/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/raian621/llm-prompting-assignment/tree/main/double/fixed.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://raian621.github.io/llm-prompting-assignment/double/fixed.html</t>
   </si>
 </sst>
 </file>
@@ -642,7 +708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -748,6 +814,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1006,8 +1076,8 @@
   </sheetPr>
   <dimension ref="A1:O906"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="I44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1713,9 +1783,13 @@
       <c r="H31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="15"/>
+      <c r="I31" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+      <c r="K31" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
@@ -2100,8 +2174,8 @@
       <c r="D51" s="25"/>
       <c r="E51" s="25"/>
       <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
+      <c r="G51" s="0"/>
+      <c r="H51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="25"/>
@@ -2109,8 +2183,8 @@
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
       <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
+      <c r="G52" s="0"/>
+      <c r="H52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="25"/>
@@ -2118,8 +2192,8 @@
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
       <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
+      <c r="G53" s="0"/>
+      <c r="H53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="25"/>
@@ -2127,8 +2201,8 @@
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
       <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
+      <c r="G54" s="0"/>
+      <c r="H54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="25"/>
@@ -2136,8 +2210,8 @@
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
       <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
+      <c r="G55" s="0"/>
+      <c r="H55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="25"/>
@@ -2145,8 +2219,8 @@
       <c r="D56" s="25"/>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
+      <c r="G56" s="0"/>
+      <c r="H56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="25"/>
@@ -2154,8 +2228,8 @@
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
+      <c r="G57" s="0"/>
+      <c r="H57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="25"/>
@@ -2163,8 +2237,8 @@
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
+      <c r="G58" s="0"/>
+      <c r="H58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="25"/>
@@ -2172,8 +2246,8 @@
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
       <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="G59" s="0"/>
+      <c r="H59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="25"/>
@@ -2181,8 +2255,8 @@
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
+      <c r="G60" s="0"/>
+      <c r="H60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="25"/>
@@ -2190,8 +2264,8 @@
       <c r="D61" s="25"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="G61" s="0"/>
+      <c r="H61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="25"/>
@@ -2199,8 +2273,8 @@
       <c r="D62" s="25"/>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
+      <c r="G62" s="0"/>
+      <c r="H62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="25"/>
@@ -2208,8 +2282,8 @@
       <c r="D63" s="25"/>
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="G63" s="0"/>
+      <c r="H63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="25"/>
@@ -2217,8 +2291,8 @@
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
       <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
+      <c r="G64" s="0"/>
+      <c r="H64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="25"/>
@@ -2226,8 +2300,8 @@
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
+      <c r="G65" s="0"/>
+      <c r="H65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="25"/>
@@ -2235,8 +2309,8 @@
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
+      <c r="G66" s="0"/>
+      <c r="H66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="25"/>
@@ -2244,8 +2318,8 @@
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
+      <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="25"/>
@@ -2253,8 +2327,8 @@
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
+      <c r="G68" s="0"/>
+      <c r="H68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="25"/>
@@ -2262,8 +2336,8 @@
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
+      <c r="G69" s="0"/>
+      <c r="H69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="25"/>
@@ -2271,8 +2345,8 @@
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
+      <c r="G70" s="0"/>
+      <c r="H70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="25"/>
@@ -2280,8 +2354,8 @@
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
+      <c r="G71" s="0"/>
+      <c r="H71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="25"/>
@@ -2289,8 +2363,8 @@
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
+      <c r="G72" s="0"/>
+      <c r="H72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="25"/>
@@ -2298,8 +2372,8 @@
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
       <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
-      <c r="H73" s="25"/>
+      <c r="G73" s="0"/>
+      <c r="H73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="25"/>
@@ -2307,8 +2381,8 @@
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
+      <c r="G74" s="0"/>
+      <c r="H74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="25"/>
@@ -2316,8 +2390,8 @@
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
-      <c r="H75" s="25"/>
+      <c r="G75" s="0"/>
+      <c r="H75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="25"/>
@@ -2325,8 +2399,8 @@
       <c r="D76" s="25"/>
       <c r="E76" s="25"/>
       <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
+      <c r="G76" s="0"/>
+      <c r="H76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="25"/>
@@ -2334,8 +2408,8 @@
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
       <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
+      <c r="G77" s="0"/>
+      <c r="H77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="25"/>
@@ -2343,8 +2417,8 @@
       <c r="D78" s="25"/>
       <c r="E78" s="25"/>
       <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
+      <c r="G78" s="0"/>
+      <c r="H78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="25"/>
@@ -2352,8 +2426,8 @@
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
       <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
+      <c r="G79" s="0"/>
+      <c r="H79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="25"/>
@@ -2361,8 +2435,8 @@
       <c r="D80" s="25"/>
       <c r="E80" s="25"/>
       <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
+      <c r="G80" s="0"/>
+      <c r="H80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="25"/>
@@ -2370,8 +2444,8 @@
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
       <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
+      <c r="G81" s="0"/>
+      <c r="H81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="25"/>
@@ -2379,8 +2453,8 @@
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
       <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="25"/>
+      <c r="G82" s="0"/>
+      <c r="H82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="25"/>
@@ -2388,8 +2462,8 @@
       <c r="D83" s="25"/>
       <c r="E83" s="25"/>
       <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
-      <c r="H83" s="25"/>
+      <c r="G83" s="0"/>
+      <c r="H83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="25"/>
@@ -2397,8 +2471,8 @@
       <c r="D84" s="25"/>
       <c r="E84" s="25"/>
       <c r="F84" s="25"/>
-      <c r="G84" s="25"/>
-      <c r="H84" s="25"/>
+      <c r="G84" s="0"/>
+      <c r="H84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="25"/>
@@ -2406,8 +2480,8 @@
       <c r="D85" s="25"/>
       <c r="E85" s="25"/>
       <c r="F85" s="25"/>
-      <c r="G85" s="25"/>
-      <c r="H85" s="25"/>
+      <c r="G85" s="0"/>
+      <c r="H85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="25"/>
@@ -2415,8 +2489,8 @@
       <c r="D86" s="25"/>
       <c r="E86" s="25"/>
       <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
-      <c r="H86" s="25"/>
+      <c r="G86" s="0"/>
+      <c r="H86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="25"/>
@@ -2424,8 +2498,8 @@
       <c r="D87" s="25"/>
       <c r="E87" s="25"/>
       <c r="F87" s="25"/>
-      <c r="G87" s="25"/>
-      <c r="H87" s="25"/>
+      <c r="G87" s="0"/>
+      <c r="H87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="25"/>
@@ -2433,8 +2507,8 @@
       <c r="D88" s="25"/>
       <c r="E88" s="25"/>
       <c r="F88" s="25"/>
-      <c r="G88" s="25"/>
-      <c r="H88" s="25"/>
+      <c r="G88" s="0"/>
+      <c r="H88" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="25"/>
@@ -2442,8 +2516,8 @@
       <c r="D89" s="25"/>
       <c r="E89" s="25"/>
       <c r="F89" s="25"/>
-      <c r="G89" s="25"/>
-      <c r="H89" s="25"/>
+      <c r="G89" s="0"/>
+      <c r="H89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="25"/>
@@ -2451,8 +2525,8 @@
       <c r="D90" s="25"/>
       <c r="E90" s="25"/>
       <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="25"/>
+      <c r="G90" s="0"/>
+      <c r="H90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="25"/>
@@ -2460,8 +2534,8 @@
       <c r="D91" s="25"/>
       <c r="E91" s="25"/>
       <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
+      <c r="G91" s="0"/>
+      <c r="H91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="25"/>
@@ -2469,8 +2543,8 @@
       <c r="D92" s="25"/>
       <c r="E92" s="25"/>
       <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
-      <c r="H92" s="25"/>
+      <c r="G92" s="0"/>
+      <c r="H92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="25"/>
@@ -2478,8 +2552,8 @@
       <c r="D93" s="25"/>
       <c r="E93" s="25"/>
       <c r="F93" s="25"/>
-      <c r="G93" s="25"/>
-      <c r="H93" s="25"/>
+      <c r="G93" s="0"/>
+      <c r="H93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="25"/>
@@ -2487,8 +2561,8 @@
       <c r="D94" s="25"/>
       <c r="E94" s="25"/>
       <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="25"/>
+      <c r="G94" s="0"/>
+      <c r="H94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="25"/>
@@ -2496,8 +2570,8 @@
       <c r="D95" s="25"/>
       <c r="E95" s="25"/>
       <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
-      <c r="H95" s="25"/>
+      <c r="G95" s="0"/>
+      <c r="H95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="25"/>
@@ -2505,8 +2579,8 @@
       <c r="D96" s="25"/>
       <c r="E96" s="25"/>
       <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
-      <c r="H96" s="25"/>
+      <c r="G96" s="0"/>
+      <c r="H96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="25"/>
@@ -2514,8 +2588,8 @@
       <c r="D97" s="25"/>
       <c r="E97" s="25"/>
       <c r="F97" s="25"/>
-      <c r="G97" s="25"/>
-      <c r="H97" s="25"/>
+      <c r="G97" s="0"/>
+      <c r="H97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="25"/>
@@ -2523,8 +2597,8 @@
       <c r="D98" s="25"/>
       <c r="E98" s="25"/>
       <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
-      <c r="H98" s="25"/>
+      <c r="G98" s="0"/>
+      <c r="H98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="25"/>
@@ -3675,8 +3749,8 @@
   </sheetPr>
   <dimension ref="A1:X895"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3799,14 +3873,14 @@
       <c r="F3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>21</v>
+      <c r="G3" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J3" s="15" t="n">
         <v>1</v>
@@ -3815,13 +3889,13 @@
         <v>33</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="2"/>
@@ -3841,10 +3915,10 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="12"/>
       <c r="I4" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>1</v>
@@ -3871,7 +3945,7 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="12"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -3897,7 +3971,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="12"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -3928,10 +4002,10 @@
         <v>25</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -4037,13 +4111,13 @@
         <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -4152,10 +4226,10 @@
         <v>25</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
@@ -4264,10 +4338,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -4376,10 +4450,10 @@
         <v>25</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -4485,13 +4559,13 @@
         <v>52</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -4598,10 +4672,10 @@
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -4710,10 +4784,10 @@
         <v>25</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -4822,10 +4896,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -4931,13 +5005,13 @@
         <v>66</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -5046,10 +5120,10 @@
         <v>25</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
@@ -5136,15 +5210,15 @@
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
-      <c r="P50" s="27"/>
-      <c r="Q50" s="27"/>
-      <c r="R50" s="27"/>
-      <c r="S50" s="27"/>
-      <c r="T50" s="27"/>
-      <c r="U50" s="27"/>
-      <c r="V50" s="27"/>
-      <c r="W50" s="27"/>
-      <c r="X50" s="27"/>
+      <c r="P50" s="28"/>
+      <c r="Q50" s="28"/>
+      <c r="R50" s="28"/>
+      <c r="S50" s="28"/>
+      <c r="T50" s="28"/>
+      <c r="U50" s="28"/>
+      <c r="V50" s="28"/>
+      <c r="W50" s="28"/>
+      <c r="X50" s="28"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
@@ -27174,43 +27248,43 @@
     <mergeCell ref="H47:H50"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId2" display="https://github.com/raian621/llm-prompting-assignment/tree/main/chatgpt/index.html"/>
-    <hyperlink ref="H3" r:id="rId3" display="https://raian621.github.io/llm-prompting-assignment/chatgpt/index.html"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://github.com/raian621/llm-prompting-assignment/tree/main/chatgpt/fixed.html"/>
+    <hyperlink ref="H3" r:id="rId3" display="https://raian621.github.io/llm-prompting-assignment/chatgpt/fixed.html"/>
     <hyperlink ref="E7" r:id="rId4" display="Ask Codi"/>
-    <hyperlink ref="G7" r:id="rId5" display="https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/index.html"/>
-    <hyperlink ref="H7" r:id="rId6" display="https://raian621.github.io/llm-prompting-assignment/ask-codi/index.html"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://github.com/raian621/llm-prompting-assignment/tree/main/ask-codi/fixed.html"/>
+    <hyperlink ref="H7" r:id="rId6" display="https://raian621.github.io/llm-prompting-assignment/ask-codi/fixed.html"/>
     <hyperlink ref="E11" r:id="rId7" display="You"/>
     <hyperlink ref="F11" r:id="rId8" display="https://you.com/search?q=I+ran+the+code+above+through+a+couple+of+online+accessibility+checkers+and+got+the+following+errors%3A...&amp;cid=c1_923b64a7-af9d-4755-82de-033a643fd86e&amp;tbm=youchat"/>
-    <hyperlink ref="G11" r:id="rId9" display="https://github.com/raian621/llm-prompting-assignment/tree/main/you/index.html"/>
-    <hyperlink ref="H11" r:id="rId10" display="https://raian621.github.io/llm-prompting-assignment/you/index.html"/>
+    <hyperlink ref="G11" r:id="rId9" display="https://github.com/raian621/llm-prompting-assignment/tree/main/you/fixed.html"/>
+    <hyperlink ref="H11" r:id="rId10" display="https://raian621.github.io/llm-prompting-assignment/you/fixed.html"/>
     <hyperlink ref="E15" r:id="rId11" display="Google Bard (Gemini)"/>
-    <hyperlink ref="G15" r:id="rId12" display="https://github.com/raian621/llm-prompting-assignment/tree/main/gemini/index.html"/>
-    <hyperlink ref="H15" r:id="rId13" display="https://raian621.github.io/llm-prompting-assignment/gemini/index.html"/>
+    <hyperlink ref="G15" r:id="rId12" display="https://github.com/raian621/llm-prompting-assignment/tree/main/gemini/fixed.html"/>
+    <hyperlink ref="H15" r:id="rId13" display="https://raian621.github.io/llm-prompting-assignment/gemini/fixed.html"/>
     <hyperlink ref="E19" r:id="rId14" display="GitHub Copilot"/>
-    <hyperlink ref="G19" r:id="rId15" display="https://github.com/raian621/llm-prompting-assignment/tree/main/github-copilot/index.html"/>
-    <hyperlink ref="H19" r:id="rId16" display="https://raian621.github.io/llm-prompting-assignment/github-copilot/index.html"/>
+    <hyperlink ref="G19" r:id="rId15" display="https://github.com/raian621/llm-prompting-assignment/tree/main/github-copilot/fixed.html"/>
+    <hyperlink ref="H19" r:id="rId16" display="https://raian621.github.io/llm-prompting-assignment/github-copilot/fixed.html"/>
     <hyperlink ref="E23" r:id="rId17" display="Amazom Whisperer"/>
-    <hyperlink ref="G23" r:id="rId18" display="https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/index.html"/>
-    <hyperlink ref="H23" r:id="rId19" display="https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/index.html"/>
+    <hyperlink ref="G23" r:id="rId18" display="https://github.com/raian621/llm-prompting-assignment/tree/main/amazon-whisperer/fixed.html"/>
+    <hyperlink ref="H23" r:id="rId19" display="https://raian621.github.io/llm-prompting-assignment/amazon-whisperer/fixed.html"/>
     <hyperlink ref="E27" r:id="rId20" display="Microsoft Copilot"/>
     <hyperlink ref="F27" r:id="rId21" display="https://copilot.microsoft.com/sl/gMszgQ8X9eC"/>
-    <hyperlink ref="G27" r:id="rId22" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/index.html"/>
-    <hyperlink ref="H27" r:id="rId23" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot.index.html"/>
+    <hyperlink ref="G27" r:id="rId22" display="https://github.com/raian621/llm-prompting-assignment/tree/main/microsoft-copilot/fixed.html"/>
+    <hyperlink ref="H27" r:id="rId23" display="https://raian621.github.io/llm-prompting-assignment/microsoft-copilot/fixed.html"/>
     <hyperlink ref="E31" r:id="rId24" display="Tabnine"/>
-    <hyperlink ref="G31" r:id="rId25" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H31" r:id="rId26" display="https://raian621.github.io/llm-prompting-assignment/tabnine/index.html"/>
+    <hyperlink ref="G31" r:id="rId25" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/fixed.html"/>
+    <hyperlink ref="H31" r:id="rId26" display="https://raian621.github.io/llm-prompting-assignment/tabnine/fixed.html"/>
     <hyperlink ref="E35" r:id="rId27" display="Codeium"/>
-    <hyperlink ref="G35" r:id="rId28" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/index.html"/>
-    <hyperlink ref="H35" r:id="rId29" display="https://raian621.github.io/llm-prompting-assignment/codeium/index.html"/>
+    <hyperlink ref="G35" r:id="rId28" display="https://github.com/raian621/llm-prompting-assignment/tree/main/codeium/fixed.html"/>
+    <hyperlink ref="H35" r:id="rId29" display="https://raian621.github.io/llm-prompting-assignment/codeium/fixed.html"/>
     <hyperlink ref="E39" r:id="rId30" display="Phind"/>
-    <hyperlink ref="G39" r:id="rId31" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/index.html"/>
-    <hyperlink ref="H39" r:id="rId32" display="https://raian621.github.io/llm-prompting-assignment/phind/index.html"/>
+    <hyperlink ref="G39" r:id="rId31" display="https://github.com/raian621/llm-prompting-assignment/tree/main/tabnine/fixed.html"/>
+    <hyperlink ref="H39" r:id="rId32" display="https://raian621.github.io/llm-prompting-assignment/phind/fixed.html"/>
     <hyperlink ref="E43" r:id="rId33" display="blackbox"/>
-    <hyperlink ref="G43" r:id="rId34" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/index.html"/>
-    <hyperlink ref="H43" r:id="rId35" display="https://raian621.github.io/llm-prompting-assignment/blackbox/index.html"/>
+    <hyperlink ref="G43" r:id="rId34" display="https://github.com/raian621/llm-prompting-assignment/tree/main/blackbox/fixed.html"/>
+    <hyperlink ref="H43" r:id="rId35" display="https://raian621.github.io/llm-prompting-assignment/blackbox/fixed.html"/>
     <hyperlink ref="E47" r:id="rId36" display="double"/>
-    <hyperlink ref="G47" r:id="rId37" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/index.html"/>
-    <hyperlink ref="H47" r:id="rId38" display="https://raian621.github.io/llm-prompting-assignment/double/index.html"/>
+    <hyperlink ref="G47" r:id="rId37" display="https://github.com/raian621/llm-prompting-assignment/tree/main/double/fixed.html"/>
+    <hyperlink ref="H47" r:id="rId38" display="https://raian621.github.io/llm-prompting-assignment/double/fixed.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>